<commit_message>
Removing DirtyPipe because it doesn't work anymore
</commit_message>
<xml_diff>
--- a/Info Linux.xlsx
+++ b/Info Linux.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josue\Documents\New folder\test123\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D8CA195-6E0E-43CF-A07F-AA906882F050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8726DEEB-948E-4BBC-8BC8-EB31433993FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{193F142C-B959-41A4-9B3D-09C676E3979B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{193F142C-B959-41A4-9B3D-09C676E3979B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -439,7 +439,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -459,7 +459,7 @@
       </c>
       <c r="E1">
         <f>COUNTA([1]!Table1511[Malware])</f>
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -471,7 +471,7 @@
       <c r="B2" s="1">
         <f>COUNTIF([1]!Table1511[Time it took for Defender to detect 
 the virus after it was downloaded?],"&lt;&gt;Didn't detect it")/E1</f>
-        <v>0.35294117647058826</v>
+        <v>0.375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating Buhti and Adding Monti
</commit_message>
<xml_diff>
--- a/Info Linux.xlsx
+++ b/Info Linux.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josue\Documents\New folder\test123\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8726DEEB-948E-4BBC-8BC8-EB31433993FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B693B7A5-19BB-431A-AB2F-80FDFF0D4DA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{193F142C-B959-41A4-9B3D-09C676E3979B}"/>
   </bookViews>
@@ -439,7 +439,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -459,7 +459,7 @@
       </c>
       <c r="E1">
         <f>COUNTA([1]!Table1511[Malware])</f>
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -471,7 +471,7 @@
       <c r="B2" s="1">
         <f>COUNTIF([1]!Table1511[Time it took for Defender to detect 
 the virus after it was downloaded?],"&lt;&gt;Didn't detect it")/E1</f>
-        <v>0.375</v>
+        <v>0.41176470588235292</v>
       </c>
     </row>
   </sheetData>

</xml_diff>